<commit_message>
Logging, Delete User, Hybrid Kalender Lic
</commit_message>
<xml_diff>
--- a/Kunden-Excel/Kunden-Excel-DRAFT.xlsx
+++ b/Kunden-Excel/Kunden-Excel-DRAFT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/630c9287b3bb8d93/03_Techniker Schule/Techniker Arbeit/WebexProv/Kunden-Excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="102" documentId="13_ncr:1_{2E292E0D-B373-416E-ABF7-3B55EED93FF2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{3F9DDBE1-7E95-134B-BD98-DF4673ED7E28}"/>
+  <xr:revisionPtr revIDLastSave="121" documentId="13_ncr:1_{2E292E0D-B373-416E-ABF7-3B55EED93FF2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{CA08AF2F-61E6-C047-B854-E5D7F2F32356}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19480" xr2:uid="{3506BBAA-2EB0-3649-9FB5-A30459E31741}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
   <si>
     <t>Name</t>
   </si>
@@ -46,15 +46,6 @@
     <t>E-Mail</t>
   </si>
   <si>
-    <t>Durchwahl</t>
-  </si>
-  <si>
-    <t>E.164</t>
-  </si>
-  <si>
-    <t>Endgerät</t>
-  </si>
-  <si>
     <t>Endgeräte</t>
   </si>
   <si>
@@ -64,49 +55,19 @@
     <t>x</t>
   </si>
   <si>
-    <t>+497117828355</t>
-  </si>
-  <si>
-    <t>Dampf</t>
-  </si>
-  <si>
     <t>Marcel</t>
   </si>
   <si>
     <t>Pludra</t>
   </si>
   <si>
-    <t>mpludra@mpludra.de</t>
-  </si>
-  <si>
-    <t>Hans</t>
-  </si>
-  <si>
-    <t>hdampf@mpludra.de</t>
-  </si>
-  <si>
-    <t>+497117828356</t>
-  </si>
-  <si>
     <t>Messaging</t>
   </si>
   <si>
-    <t>Calling</t>
-  </si>
-  <si>
-    <t>Bla</t>
-  </si>
-  <si>
-    <t>bla@mpludra.de</t>
-  </si>
-  <si>
-    <t>+49171304534</t>
-  </si>
-  <si>
-    <t>Bla1</t>
-  </si>
-  <si>
-    <t>Blala1</t>
+    <t>Bla10@mpludra.de</t>
+  </si>
+  <si>
+    <t>Kalender (Exchange)</t>
   </si>
 </sst>
 </file>
@@ -165,10 +126,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -499,389 +459,217 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC3540F1-6548-7943-9FC4-7B110902D3A7}">
-  <dimension ref="A1:I40"/>
+  <dimension ref="A1:G39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="15.83203125" customWidth="1"/>
     <col min="3" max="3" width="21.6640625" customWidth="1"/>
-    <col min="5" max="5" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="13" style="4" customWidth="1"/>
-    <col min="8" max="8" width="10.83203125" style="4"/>
+    <col min="4" max="5" width="13" style="3" customWidth="1"/>
+    <col min="6" max="6" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="G1" s="7" t="s">
+      <c r="F1" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="6"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="I1" s="6" t="s">
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2">
-        <v>55</v>
-      </c>
       <c r="E2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3">
-        <v>56</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4">
-        <v>54</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" t="str">
-        <f>A5&amp;"@mpludra.de"</f>
-        <v>Bla1@mpludra.de</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C3" s="1"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C4" s="1"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D5" s="2"/>
       <c r="E5" s="2"/>
-      <c r="F5" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D6" s="2"/>
       <c r="E6" s="2"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D7" s="2"/>
       <c r="E7" s="2"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D8" s="2"/>
       <c r="E8" s="2"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D9" s="2"/>
       <c r="E9" s="2"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D10" s="2"/>
       <c r="E10" s="2"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D11" s="2"/>
       <c r="E11" s="2"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D12" s="2"/>
       <c r="E12" s="2"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D13" s="2"/>
       <c r="E13" s="2"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D14" s="2"/>
       <c r="E14" s="2"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D15" s="2"/>
       <c r="E15" s="2"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D16" s="2"/>
       <c r="E16" s="2"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-    </row>
-    <row r="17" spans="5:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D17" s="2"/>
       <c r="E17" s="2"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-    </row>
-    <row r="18" spans="5:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D18" s="2"/>
       <c r="E18" s="2"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-    </row>
-    <row r="19" spans="5:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D19" s="2"/>
       <c r="E19" s="2"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
-    </row>
-    <row r="20" spans="5:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D20" s="2"/>
       <c r="E20" s="2"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
-    </row>
-    <row r="21" spans="5:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D21" s="2"/>
       <c r="E21" s="2"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
-    </row>
-    <row r="22" spans="5:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D22" s="2"/>
       <c r="E22" s="2"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
-    </row>
-    <row r="23" spans="5:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D23" s="2"/>
       <c r="E23" s="2"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
-      <c r="I23" s="3"/>
-    </row>
-    <row r="24" spans="5:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D24" s="2"/>
       <c r="E24" s="2"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-      <c r="H24" s="3"/>
-      <c r="I24" s="3"/>
-    </row>
-    <row r="25" spans="5:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D25" s="2"/>
       <c r="E25" s="2"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
-      <c r="H25" s="3"/>
-      <c r="I25" s="3"/>
-    </row>
-    <row r="26" spans="5:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D26" s="2"/>
       <c r="E26" s="2"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-      <c r="H26" s="3"/>
-      <c r="I26" s="3"/>
-    </row>
-    <row r="27" spans="5:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D27" s="2"/>
       <c r="E27" s="2"/>
-      <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
-      <c r="H27" s="3"/>
-      <c r="I27" s="3"/>
-    </row>
-    <row r="28" spans="5:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D28" s="2"/>
       <c r="E28" s="2"/>
-      <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
-      <c r="H28" s="3"/>
-      <c r="I28" s="3"/>
-    </row>
-    <row r="29" spans="5:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="29" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D29" s="2"/>
       <c r="E29" s="2"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
-      <c r="H29" s="3"/>
-      <c r="I29" s="3"/>
-    </row>
-    <row r="30" spans="5:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D30" s="2"/>
       <c r="E30" s="2"/>
-      <c r="F30" s="3"/>
-      <c r="G30" s="3"/>
-      <c r="H30" s="3"/>
-      <c r="I30" s="3"/>
-    </row>
-    <row r="31" spans="5:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="31" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D31" s="2"/>
       <c r="E31" s="2"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="3"/>
-      <c r="H31" s="3"/>
-      <c r="I31" s="3"/>
-    </row>
-    <row r="32" spans="5:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D32" s="2"/>
       <c r="E32" s="2"/>
-      <c r="F32" s="3"/>
-      <c r="G32" s="3"/>
-      <c r="H32" s="3"/>
-      <c r="I32" s="3"/>
-    </row>
-    <row r="33" spans="5:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="33" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D33" s="2"/>
       <c r="E33" s="2"/>
-      <c r="F33" s="3"/>
-      <c r="G33" s="3"/>
-      <c r="H33" s="3"/>
-      <c r="I33" s="3"/>
-    </row>
-    <row r="34" spans="5:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="34" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D34" s="2"/>
       <c r="E34" s="2"/>
-      <c r="F34" s="3"/>
-      <c r="G34" s="3"/>
-      <c r="H34" s="3"/>
-      <c r="I34" s="3"/>
-    </row>
-    <row r="35" spans="5:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="35" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D35" s="2"/>
       <c r="E35" s="2"/>
-      <c r="F35" s="3"/>
-      <c r="G35" s="3"/>
-      <c r="H35" s="3"/>
-      <c r="I35" s="3"/>
-    </row>
-    <row r="36" spans="5:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="36" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D36" s="2"/>
       <c r="E36" s="2"/>
-      <c r="F36" s="3"/>
-      <c r="G36" s="3"/>
-      <c r="H36" s="3"/>
-      <c r="I36" s="3"/>
-    </row>
-    <row r="37" spans="5:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="37" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D37" s="2"/>
       <c r="E37" s="2"/>
-      <c r="F37" s="3"/>
-      <c r="G37" s="3"/>
-      <c r="H37" s="3"/>
-      <c r="I37" s="3"/>
-    </row>
-    <row r="38" spans="5:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="38" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D38" s="2"/>
       <c r="E38" s="2"/>
-      <c r="F38" s="3"/>
-      <c r="G38" s="3"/>
-      <c r="H38" s="3"/>
-      <c r="I38" s="3"/>
-    </row>
-    <row r="39" spans="5:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="39" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D39" s="2"/>
       <c r="E39" s="2"/>
-      <c r="F39" s="3"/>
-      <c r="G39" s="3"/>
-      <c r="H39" s="3"/>
-      <c r="I39" s="3"/>
-    </row>
-    <row r="40" spans="5:9" x14ac:dyDescent="0.2">
-      <c r="E40" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{1B47DF7F-1066-4387-B1D0-34547DE1F0AA}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{D762FB3E-B854-4144-8312-5FE71228982D}"/>
-    <hyperlink ref="C4" r:id="rId3" xr:uid="{1E13371E-91C1-CB4D-ACA8-0AB7EC88FA26}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -902,7 +690,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Durchlaufen der Excel angepasst
</commit_message>
<xml_diff>
--- a/Kunden-Excel/Kunden-Excel-DRAFT.xlsx
+++ b/Kunden-Excel/Kunden-Excel-DRAFT.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/630c9287b3bb8d93/03_Techniker Schule/Techniker Arbeit/WebexProv/Kunden-Excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marcel\Documents\WebexProv\Kunden-Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="121" documentId="13_ncr:1_{2E292E0D-B373-416E-ABF7-3B55EED93FF2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{CA08AF2F-61E6-C047-B854-E5D7F2F32356}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19480" xr2:uid="{3506BBAA-2EB0-3649-9FB5-A30459E31741}"/>
+    <workbookView xWindow="0" yWindow="495" windowWidth="33600" windowHeight="19485"/>
   </bookViews>
   <sheets>
     <sheet name="Daten" sheetId="1" r:id="rId1"/>
     <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
   <si>
     <t>Name</t>
   </si>
@@ -68,12 +67,90 @@
   </si>
   <si>
     <t>Kalender (Exchange)</t>
+  </si>
+  <si>
+    <t>test1</t>
+  </si>
+  <si>
+    <t>test2</t>
+  </si>
+  <si>
+    <t>test3</t>
+  </si>
+  <si>
+    <t>test4</t>
+  </si>
+  <si>
+    <t>test5</t>
+  </si>
+  <si>
+    <t>test6</t>
+  </si>
+  <si>
+    <t>test7</t>
+  </si>
+  <si>
+    <t>test8</t>
+  </si>
+  <si>
+    <t>test9</t>
+  </si>
+  <si>
+    <t>test10</t>
+  </si>
+  <si>
+    <t>test11</t>
+  </si>
+  <si>
+    <t>test12</t>
+  </si>
+  <si>
+    <t>test13</t>
+  </si>
+  <si>
+    <t>test14</t>
+  </si>
+  <si>
+    <t>test15</t>
+  </si>
+  <si>
+    <t>test16</t>
+  </si>
+  <si>
+    <t>test17</t>
+  </si>
+  <si>
+    <t>test18</t>
+  </si>
+  <si>
+    <t>test19</t>
+  </si>
+  <si>
+    <t>test20</t>
+  </si>
+  <si>
+    <t>test21</t>
+  </si>
+  <si>
+    <t>test22</t>
+  </si>
+  <si>
+    <t>test23</t>
+  </si>
+  <si>
+    <t>test24</t>
+  </si>
+  <si>
+    <t>test25</t>
+  </si>
+  <si>
+    <t>test26</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -458,23 +535,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC3540F1-6548-7943-9FC4-7B110902D3A7}">
-  <dimension ref="A1:G39"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G198"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.83203125" customWidth="1"/>
-    <col min="3" max="3" width="21.6640625" customWidth="1"/>
+    <col min="2" max="2" width="15.875" customWidth="1"/>
+    <col min="3" max="3" width="21.625" customWidth="1"/>
     <col min="4" max="5" width="13" style="3" customWidth="1"/>
-    <col min="6" max="6" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.33203125" customWidth="1"/>
+    <col min="6" max="6" width="18.875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -495,7 +572,7 @@
       </c>
       <c r="G1" s="6"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -516,199 +593,641 @@
       </c>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C3" s="1"/>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="str">
+        <f>A3</f>
+        <v>test1</v>
+      </c>
+      <c r="C3" s="1" t="str">
+        <f>A3&amp;"@mpludra.de"</f>
+        <v>test1@mpludra.de</v>
+      </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C4" s="1"/>
+      <c r="F3" s="2"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="str">
+        <f t="shared" ref="B4:B28" si="0">A4</f>
+        <v>test2</v>
+      </c>
+      <c r="C4" s="1" t="str">
+        <f t="shared" ref="C4:C28" si="1">A4&amp;"@mpludra.de"</f>
+        <v>test2@mpludra.de</v>
+      </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F4" s="2"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="str">
+        <f t="shared" si="0"/>
+        <v>test3</v>
+      </c>
+      <c r="C5" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>test3@mpludra.de</v>
+      </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F5" s="2"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="str">
+        <f t="shared" si="0"/>
+        <v>test4</v>
+      </c>
+      <c r="C6" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>test4@mpludra.de</v>
+      </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F6" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="str">
+        <f t="shared" si="0"/>
+        <v>test5</v>
+      </c>
+      <c r="C7" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>test5@mpludra.de</v>
+      </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="str">
+        <f t="shared" si="0"/>
+        <v>test6</v>
+      </c>
+      <c r="C8" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>test6@mpludra.de</v>
+      </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F8" s="2"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" t="str">
+        <f t="shared" si="0"/>
+        <v>test7</v>
+      </c>
+      <c r="C9" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>test7@mpludra.de</v>
+      </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F9" s="2"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" t="str">
+        <f t="shared" si="0"/>
+        <v>test8</v>
+      </c>
+      <c r="C10" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>test8@mpludra.de</v>
+      </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F10" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" t="str">
+        <f t="shared" si="0"/>
+        <v>test9</v>
+      </c>
+      <c r="C11" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>test9@mpludra.de</v>
+      </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F11" s="2"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" t="str">
+        <f t="shared" si="0"/>
+        <v>test10</v>
+      </c>
+      <c r="C12" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>test10@mpludra.de</v>
+      </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" t="str">
+        <f t="shared" si="0"/>
+        <v>test11</v>
+      </c>
+      <c r="C13" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>test11@mpludra.de</v>
+      </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F13" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" t="str">
+        <f t="shared" si="0"/>
+        <v>test12</v>
+      </c>
+      <c r="C14" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>test12@mpludra.de</v>
+      </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" t="str">
+        <f t="shared" si="0"/>
+        <v>test13</v>
+      </c>
+      <c r="C15" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>test13@mpludra.de</v>
+      </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F15" s="2"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" t="str">
+        <f t="shared" si="0"/>
+        <v>test14</v>
+      </c>
+      <c r="C16" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>test14@mpludra.de</v>
+      </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
-    </row>
-    <row r="17" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="F16" s="2"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" t="str">
+        <f t="shared" si="0"/>
+        <v>test15</v>
+      </c>
+      <c r="C17" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>test15@mpludra.de</v>
+      </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
-    </row>
-    <row r="18" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="F17" s="2"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" t="str">
+        <f t="shared" si="0"/>
+        <v>test16</v>
+      </c>
+      <c r="C18" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>test16@mpludra.de</v>
+      </c>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
-    </row>
-    <row r="19" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="F18" s="2"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" t="str">
+        <f t="shared" si="0"/>
+        <v>test17</v>
+      </c>
+      <c r="C19" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>test17@mpludra.de</v>
+      </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
-    </row>
-    <row r="20" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="F19" s="2"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20" t="str">
+        <f t="shared" si="0"/>
+        <v>test18</v>
+      </c>
+      <c r="C20" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>test18@mpludra.de</v>
+      </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
-    </row>
-    <row r="21" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="F20" s="2"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" t="str">
+        <f t="shared" si="0"/>
+        <v>test19</v>
+      </c>
+      <c r="C21" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>test19@mpludra.de</v>
+      </c>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
-    </row>
-    <row r="22" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="F21" s="2"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" t="str">
+        <f t="shared" si="0"/>
+        <v>test20</v>
+      </c>
+      <c r="C22" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>test20@mpludra.de</v>
+      </c>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
-    </row>
-    <row r="23" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="F22" s="2"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>31</v>
+      </c>
+      <c r="B23" t="str">
+        <f t="shared" si="0"/>
+        <v>test21</v>
+      </c>
+      <c r="C23" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>test21@mpludra.de</v>
+      </c>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
-    </row>
-    <row r="24" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="F23" s="2"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>32</v>
+      </c>
+      <c r="B24" t="str">
+        <f t="shared" si="0"/>
+        <v>test22</v>
+      </c>
+      <c r="C24" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>test22@mpludra.de</v>
+      </c>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
-    </row>
-    <row r="25" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="F24" s="2"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>33</v>
+      </c>
+      <c r="B25" t="str">
+        <f t="shared" si="0"/>
+        <v>test23</v>
+      </c>
+      <c r="C25" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>test23@mpludra.de</v>
+      </c>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
-    </row>
-    <row r="26" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="F25" s="2"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>34</v>
+      </c>
+      <c r="B26" t="str">
+        <f t="shared" si="0"/>
+        <v>test24</v>
+      </c>
+      <c r="C26" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>test24@mpludra.de</v>
+      </c>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
-    </row>
-    <row r="27" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="F26" s="2"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>35</v>
+      </c>
+      <c r="B27" t="str">
+        <f t="shared" si="0"/>
+        <v>test25</v>
+      </c>
+      <c r="C27" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>test25@mpludra.de</v>
+      </c>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
-    </row>
-    <row r="28" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="F27" s="2"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28" t="str">
+        <f t="shared" si="0"/>
+        <v>test26</v>
+      </c>
+      <c r="C28" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>test26@mpludra.de</v>
+      </c>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
-    </row>
-    <row r="29" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-    </row>
-    <row r="30" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-    </row>
-    <row r="31" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-    </row>
-    <row r="32" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-    </row>
-    <row r="33" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
-    </row>
-    <row r="34" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
-    </row>
-    <row r="35" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
-    </row>
-    <row r="36" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D36" s="2"/>
-      <c r="E36" s="2"/>
-    </row>
-    <row r="37" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D37" s="2"/>
-      <c r="E37" s="2"/>
-    </row>
-    <row r="38" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D38" s="2"/>
-      <c r="E38" s="2"/>
-    </row>
-    <row r="39" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D39" s="2"/>
-      <c r="E39" s="2"/>
-    </row>
+      <c r="F28" s="2"/>
+    </row>
+    <row r="29" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="33" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="35" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="44" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="49" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="50" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="55" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="56" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="57" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="58" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="59" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="60" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="61" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="62" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="63" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="64" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="65" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="66" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="67" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="68" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="69" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="70" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="71" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="72" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="73" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="74" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="75" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="76" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="77" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="78" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="79" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="80" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="81" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="82" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="83" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="84" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="85" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="86" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="87" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="88" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="89" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="90" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="91" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="92" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="93" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="94" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="95" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="96" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="97" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="98" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="99" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="100" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="101" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="102" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="103" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="104" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="105" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="106" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="107" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="108" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="109" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="110" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="111" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="112" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="113" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="114" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="115" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="116" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="117" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="118" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="119" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="120" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="121" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="122" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="123" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="124" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="125" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="126" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="127" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="128" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="129" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="130" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="131" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="132" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="133" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="134" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="135" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="136" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="137" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="138" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="139" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="140" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="141" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="142" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="143" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="144" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="145" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="146" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="147" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="148" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="149" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="150" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="151" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="152" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="153" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="154" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="155" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="156" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="157" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="158" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="159" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="160" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="161" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="162" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="163" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="164" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="165" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="166" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="167" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="168" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="169" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="170" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="171" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="172" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="173" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="174" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="175" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="176" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="177" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="178" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="179" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="180" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="181" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="182" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="183" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="184" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="185" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="186" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="187" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="188" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="189" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="190" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="191" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="192" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="193" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="194" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="195" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="196" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="197" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="198" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{1B47DF7F-1066-4387-B1D0-34547DE1F0AA}"/>
+    <hyperlink ref="C2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{523ED8D9-46D2-0B4D-8E3C-559EF5634E3B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>8841</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>8851</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>8845</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>8865</v>
       </c>

</xml_diff>